<commit_message>
First imlementation for finding the hazard rate
</commit_message>
<xml_diff>
--- a/curvas2.xlsx
+++ b/curvas2.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eliah\Documents\Banorte\swap-valuation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D9DB31-95BB-405A-93FA-4D8EFF469BFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD76DBD-A065-448F-9DD3-B19B31F9EB62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F5E3D12E-4134-40E4-AC8B-4E780EB244CF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Curva" sheetId="2" r:id="rId1"/>
-    <sheet name="Aux" sheetId="1" r:id="rId2"/>
+    <sheet name="Curva" sheetId="3" r:id="rId1"/>
+    <sheet name="Curva anterior" sheetId="2" r:id="rId2"/>
+    <sheet name="Aux" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>12 MO</t>
   </si>
@@ -145,13 +146,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -162,7 +176,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -170,13 +184,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -195,9 +236,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -235,7 +276,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -341,7 +382,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -483,18 +524,308 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD5D2C3-092C-4B1D-8867-40AD9CEB184C}">
+  <dimension ref="A1:B34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="5">
+        <v>45954</v>
+      </c>
+      <c r="B2" s="4">
+        <v>3.9891399999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="3">
+        <v>45965</v>
+      </c>
+      <c r="B3" s="4">
+        <v>3.9891399999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="3">
+        <v>45973</v>
+      </c>
+      <c r="B4" s="4">
+        <v>3.9596</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="3">
+        <v>45979</v>
+      </c>
+      <c r="B5" s="4">
+        <v>3.9491900000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="3">
+        <v>45989</v>
+      </c>
+      <c r="B6" s="4">
+        <v>3.9392299999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="3">
+        <v>46020</v>
+      </c>
+      <c r="B7" s="4">
+        <v>3.8572199999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="3">
+        <v>46050</v>
+      </c>
+      <c r="B8" s="4">
+        <v>3.7948400000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="3">
+        <v>46080</v>
+      </c>
+      <c r="B9" s="4">
+        <v>3.7295699999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="3">
+        <v>46111</v>
+      </c>
+      <c r="B10" s="4">
+        <v>3.6789200000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="3">
+        <v>46140</v>
+      </c>
+      <c r="B11" s="4">
+        <v>3.6342400000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="3">
+        <v>46170</v>
+      </c>
+      <c r="B12" s="4">
+        <v>3.5933000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="3">
+        <v>46202</v>
+      </c>
+      <c r="B13" s="4">
+        <v>3.5539200000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="3">
+        <v>46231</v>
+      </c>
+      <c r="B14" s="4">
+        <v>3.5169600000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="3">
+        <v>46262</v>
+      </c>
+      <c r="B15" s="4">
+        <v>3.47776</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="3">
+        <v>46293</v>
+      </c>
+      <c r="B16" s="4">
+        <v>3.4430800000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="3">
+        <v>46323</v>
+      </c>
+      <c r="B17" s="4">
+        <v>3.41066</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="3">
+        <v>46505</v>
+      </c>
+      <c r="B18" s="4">
+        <v>3.2620200000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="3">
+        <v>46688</v>
+      </c>
+      <c r="B19" s="4">
+        <v>3.1904300000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="3">
+        <v>47056</v>
+      </c>
+      <c r="B20" s="4">
+        <v>3.1570299999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="3">
+        <v>47420</v>
+      </c>
+      <c r="B21" s="4">
+        <v>3.1829900000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="3">
+        <v>47784</v>
+      </c>
+      <c r="B22" s="4">
+        <v>3.2283400000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="3">
+        <v>48149</v>
+      </c>
+      <c r="B23" s="4">
+        <v>3.2840099999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="3">
+        <v>48515</v>
+      </c>
+      <c r="B24" s="4">
+        <v>3.3460200000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="3">
+        <v>48880</v>
+      </c>
+      <c r="B25" s="4">
+        <v>3.40883</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="3">
+        <v>49247</v>
+      </c>
+      <c r="B26" s="4">
+        <v>3.47241</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="3">
+        <v>49611</v>
+      </c>
+      <c r="B27" s="4">
+        <v>3.5341</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="3">
+        <v>50341</v>
+      </c>
+      <c r="B28" s="4">
+        <v>3.65178</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="3">
+        <v>51438</v>
+      </c>
+      <c r="B29" s="4">
+        <v>3.7943600000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="3">
+        <v>53265</v>
+      </c>
+      <c r="B30" s="4">
+        <v>3.9108800000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="3">
+        <v>55089</v>
+      </c>
+      <c r="B31" s="4">
+        <v>3.9050600000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="3">
+        <v>56915</v>
+      </c>
+      <c r="B32" s="4">
+        <v>3.8376899999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="3">
+        <v>60568</v>
+      </c>
+      <c r="B33" s="4">
+        <v>3.6242100000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="3">
+        <v>64220</v>
+      </c>
+      <c r="B34" s="4">
+        <v>3.3721199999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7D5EA78-07BD-4C95-8DD4-34791235D2EA}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -513,7 +844,7 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <f ca="1">+Aux!B1</f>
-        <v>45178</v>
+        <v>45954</v>
       </c>
       <c r="B2">
         <v>5.3720600000000003</v>
@@ -522,7 +853,7 @@
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <f ca="1">Aux!D3</f>
-        <v>45187</v>
+        <v>45961</v>
       </c>
       <c r="B3">
         <v>5.3720600000000003</v>
@@ -531,7 +862,7 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <f ca="1">Aux!D4</f>
-        <v>45194</v>
+        <v>45968</v>
       </c>
       <c r="B4">
         <v>5.3814599999999997</v>
@@ -540,7 +871,7 @@
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <f ca="1">Aux!D5</f>
-        <v>45201</v>
+        <v>45975</v>
       </c>
       <c r="B5">
         <v>5.3869100000000003</v>
@@ -549,7 +880,7 @@
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <f ca="1">Aux!D6</f>
-        <v>45208</v>
+        <v>45985</v>
       </c>
       <c r="B6">
         <v>5.3905599999999998</v>
@@ -558,7 +889,7 @@
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <f ca="1">Aux!D7</f>
-        <v>45239</v>
+        <v>46015</v>
       </c>
       <c r="B7">
         <v>5.4125300000000003</v>
@@ -567,7 +898,7 @@
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <f ca="1">Aux!D8</f>
-        <v>45271</v>
+        <v>46048</v>
       </c>
       <c r="B8">
         <v>5.44245</v>
@@ -576,7 +907,7 @@
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <f ca="1">Aux!D9</f>
-        <v>45300</v>
+        <v>46077</v>
       </c>
       <c r="B9">
         <v>5.4572599999999998</v>
@@ -585,7 +916,7 @@
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <f ca="1">Aux!D10</f>
-        <v>45331</v>
+        <v>46105</v>
       </c>
       <c r="B10">
         <v>5.4647199999999998</v>
@@ -594,7 +925,7 @@
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <f ca="1">Aux!D11</f>
-        <v>45362</v>
+        <v>46136</v>
       </c>
       <c r="B11">
         <v>5.4645599999999996</v>
@@ -603,7 +934,7 @@
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <f ca="1">Aux!D12</f>
-        <v>45391</v>
+        <v>46167</v>
       </c>
       <c r="B12">
         <v>5.4585699999999999</v>
@@ -612,7 +943,7 @@
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <f ca="1">Aux!D13</f>
-        <v>45421</v>
+        <v>46197</v>
       </c>
       <c r="B13">
         <v>5.4466799999999997</v>
@@ -621,7 +952,7 @@
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <f ca="1">Aux!D14</f>
-        <v>45453</v>
+        <v>46227</v>
       </c>
       <c r="B14">
         <v>5.4305099999999999</v>
@@ -630,7 +961,7 @@
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <f ca="1">Aux!D15</f>
-        <v>45482</v>
+        <v>46258</v>
       </c>
       <c r="B15">
         <v>5.4050900000000004</v>
@@ -639,7 +970,7 @@
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <f ca="1">Aux!D16</f>
-        <v>45513</v>
+        <v>46289</v>
       </c>
       <c r="B16">
         <v>5.3783099999999999</v>
@@ -648,7 +979,7 @@
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <f ca="1">Aux!D17</f>
-        <v>45544</v>
+        <v>46321</v>
       </c>
       <c r="B17">
         <v>5.3464</v>
@@ -657,7 +988,7 @@
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <f ca="1">Aux!D18</f>
-        <v>45726</v>
+        <v>46503</v>
       </c>
       <c r="B18">
         <v>5.09497</v>
@@ -666,7 +997,7 @@
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <f ca="1">Aux!D19</f>
-        <v>45909</v>
+        <v>46685</v>
       </c>
       <c r="B19">
         <v>4.8235000000000001</v>
@@ -675,7 +1006,7 @@
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <f ca="1">Aux!D20</f>
-        <v>46274</v>
+        <v>47050</v>
       </c>
       <c r="B20">
         <v>4.4600299999999997</v>
@@ -684,7 +1015,7 @@
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <f ca="1">Aux!D21</f>
-        <v>46639</v>
+        <v>47415</v>
       </c>
       <c r="B21">
         <v>4.2483599999999999</v>
@@ -693,7 +1024,7 @@
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <f ca="1">Aux!D22</f>
-        <v>47007</v>
+        <v>47780</v>
       </c>
       <c r="B22">
         <v>4.1230700000000002</v>
@@ -702,7 +1033,7 @@
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <f ca="1">Aux!D23</f>
-        <v>47371</v>
+        <v>48145</v>
       </c>
       <c r="B23">
         <v>4.0446200000000001</v>
@@ -711,7 +1042,7 @@
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <f ca="1">Aux!D24</f>
-        <v>47735</v>
+        <v>48512</v>
       </c>
       <c r="B24">
         <v>3.98935</v>
@@ -720,7 +1051,7 @@
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <f ca="1">Aux!D25</f>
-        <v>48100</v>
+        <v>48876</v>
       </c>
       <c r="B25">
         <v>3.9533800000000001</v>
@@ -729,7 +1060,7 @@
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <f ca="1">Aux!D26</f>
-        <v>48466</v>
+        <v>49241</v>
       </c>
       <c r="B26">
         <v>3.9308800000000002</v>
@@ -738,7 +1069,7 @@
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <f ca="1">Aux!D27</f>
-        <v>48831</v>
+        <v>49606</v>
       </c>
       <c r="B27">
         <v>3.91513</v>
@@ -747,7 +1078,7 @@
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <f ca="1">Aux!D28</f>
-        <v>49562</v>
+        <v>50339</v>
       </c>
       <c r="B28">
         <v>3.9041800000000002</v>
@@ -756,7 +1087,7 @@
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <f ca="1">Aux!D29</f>
-        <v>50657</v>
+        <v>51433</v>
       </c>
       <c r="B29">
         <v>3.9005899999999998</v>
@@ -765,7 +1096,7 @@
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <f ca="1">Aux!D30</f>
-        <v>52483</v>
+        <v>53259</v>
       </c>
       <c r="B30">
         <v>3.83222</v>
@@ -774,7 +1105,7 @@
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <f ca="1">Aux!D31</f>
-        <v>54310</v>
+        <v>55085</v>
       </c>
       <c r="B31">
         <v>3.67354</v>
@@ -783,7 +1114,7 @@
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <f ca="1">Aux!D32</f>
-        <v>56136</v>
+        <v>56912</v>
       </c>
       <c r="B32">
         <v>3.5152600000000001</v>
@@ -792,7 +1123,7 @@
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <f ca="1">Aux!D33</f>
-        <v>59789</v>
+        <v>60566</v>
       </c>
       <c r="B33">
         <v>3.1892800000000001</v>
@@ -801,7 +1132,7 @@
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <f ca="1">Aux!D34</f>
-        <v>63443</v>
+        <v>64216</v>
       </c>
       <c r="B34">
         <v>2.8502900000000002</v>
@@ -812,12 +1143,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E396DB93-9A92-496F-80C2-F7F03073A5F4}">
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -828,7 +1159,7 @@
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" s="1">
         <f ca="1">TODAY()</f>
-        <v>45178</v>
+        <v>45954</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -837,15 +1168,15 @@
       </c>
       <c r="C3" s="1">
         <f ca="1">+B1+7</f>
-        <v>45185</v>
+        <v>45961</v>
       </c>
       <c r="D3" s="1">
         <f ca="1">WORKDAY(C3-1,1)</f>
-        <v>45187</v>
+        <v>45961</v>
       </c>
       <c r="E3">
         <f ca="1">WEEKDAY(D3, 1)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -854,15 +1185,15 @@
       </c>
       <c r="C4" s="1">
         <f ca="1">C3+7</f>
-        <v>45192</v>
+        <v>45968</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" ref="D4:D34" ca="1" si="0">WORKDAY(C4-1,1)</f>
-        <v>45194</v>
+        <v>45968</v>
       </c>
       <c r="E4">
         <f t="shared" ref="E4:E34" ca="1" si="1">WEEKDAY(D4, 1)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -871,15 +1202,15 @@
       </c>
       <c r="C5" s="1">
         <f ca="1">C4+7</f>
-        <v>45199</v>
+        <v>45975</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>45201</v>
+        <v>45975</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -891,11 +1222,11 @@
       </c>
       <c r="C6" s="1">
         <f ca="1">EDATE($B$1, A6)</f>
-        <v>45208</v>
+        <v>45985</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>45208</v>
+        <v>45985</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
@@ -911,15 +1242,15 @@
       </c>
       <c r="C7" s="1">
         <f t="shared" ref="C7:C18" ca="1" si="2">EDATE($B$1, A7)</f>
-        <v>45239</v>
+        <v>46015</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>45239</v>
+        <v>46015</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -931,11 +1262,11 @@
       </c>
       <c r="C8" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>45269</v>
+        <v>46046</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>45271</v>
+        <v>46048</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
@@ -951,11 +1282,11 @@
       </c>
       <c r="C9" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>45300</v>
+        <v>46077</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>45300</v>
+        <v>46077</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
@@ -971,15 +1302,15 @@
       </c>
       <c r="C10" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>45331</v>
+        <v>46105</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>45331</v>
+        <v>46105</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -991,15 +1322,15 @@
       </c>
       <c r="C11" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>45360</v>
+        <v>46136</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>45362</v>
+        <v>46136</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -1011,15 +1342,15 @@
       </c>
       <c r="C12" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>45391</v>
+        <v>46166</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>45391</v>
+        <v>46167</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -1031,15 +1362,15 @@
       </c>
       <c r="C13" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>45421</v>
+        <v>46197</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>45421</v>
+        <v>46197</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -1051,15 +1382,15 @@
       </c>
       <c r="C14" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>45452</v>
+        <v>46227</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>45453</v>
+        <v>46227</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -1071,15 +1402,15 @@
       </c>
       <c r="C15" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>45482</v>
+        <v>46258</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>45482</v>
+        <v>46258</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -1091,15 +1422,15 @@
       </c>
       <c r="C16" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>45513</v>
+        <v>46289</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>45513</v>
+        <v>46289</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -1111,11 +1442,11 @@
       </c>
       <c r="C17" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>45544</v>
+        <v>46319</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>45544</v>
+        <v>46321</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
@@ -1131,11 +1462,11 @@
       </c>
       <c r="C18" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>45725</v>
+        <v>46501</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>45726</v>
+        <v>46503</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
@@ -1151,15 +1482,15 @@
       </c>
       <c r="C19" s="1">
         <f ca="1">EDATE($B$1, A19*12)</f>
-        <v>45909</v>
+        <v>46684</v>
       </c>
       <c r="D19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>45909</v>
+        <v>46685</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -1171,15 +1502,15 @@
       </c>
       <c r="C20" s="1">
         <f t="shared" ref="C20:C34" ca="1" si="3">EDATE($B$1, A20*12)</f>
-        <v>46274</v>
+        <v>47050</v>
       </c>
       <c r="D20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>46274</v>
+        <v>47050</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -1191,15 +1522,15 @@
       </c>
       <c r="C21" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>46639</v>
+        <v>47415</v>
       </c>
       <c r="D21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>46639</v>
+        <v>47415</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -1211,15 +1542,15 @@
       </c>
       <c r="C22" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>47005</v>
+        <v>47780</v>
       </c>
       <c r="D22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>47007</v>
+        <v>47780</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -1231,15 +1562,15 @@
       </c>
       <c r="C23" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>47370</v>
+        <v>48145</v>
       </c>
       <c r="D23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>47371</v>
+        <v>48145</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -1251,11 +1582,11 @@
       </c>
       <c r="C24" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>47735</v>
+        <v>48511</v>
       </c>
       <c r="D24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>47735</v>
+        <v>48512</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="1"/>
@@ -1271,15 +1602,15 @@
       </c>
       <c r="C25" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>48100</v>
+        <v>48876</v>
       </c>
       <c r="D25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>48100</v>
+        <v>48876</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -1291,15 +1622,15 @@
       </c>
       <c r="C26" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>48466</v>
+        <v>49241</v>
       </c>
       <c r="D26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>48466</v>
+        <v>49241</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -1311,15 +1642,15 @@
       </c>
       <c r="C27" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>48831</v>
+        <v>49606</v>
       </c>
       <c r="D27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>48831</v>
+        <v>49606</v>
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -1331,11 +1662,11 @@
       </c>
       <c r="C28" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>49561</v>
+        <v>50337</v>
       </c>
       <c r="D28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>49562</v>
+        <v>50339</v>
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="1"/>
@@ -1351,15 +1682,15 @@
       </c>
       <c r="C29" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>50657</v>
+        <v>51433</v>
       </c>
       <c r="D29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>50657</v>
+        <v>51433</v>
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -1371,15 +1702,15 @@
       </c>
       <c r="C30" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>52483</v>
+        <v>53259</v>
       </c>
       <c r="D30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>52483</v>
+        <v>53259</v>
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -1391,15 +1722,15 @@
       </c>
       <c r="C31" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>54310</v>
+        <v>55085</v>
       </c>
       <c r="D31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>54310</v>
+        <v>55085</v>
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -1411,15 +1742,15 @@
       </c>
       <c r="C32" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>56136</v>
+        <v>56911</v>
       </c>
       <c r="D32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>56136</v>
+        <v>56912</v>
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -1431,11 +1762,11 @@
       </c>
       <c r="C33" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>59788</v>
+        <v>60564</v>
       </c>
       <c r="D33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>59789</v>
+        <v>60566</v>
       </c>
       <c r="E33">
         <f t="shared" ca="1" si="1"/>
@@ -1451,15 +1782,15 @@
       </c>
       <c r="C34" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>63441</v>
+        <v>64216</v>
       </c>
       <c r="D34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>63443</v>
+        <v>64216</v>
       </c>
       <c r="E34">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>